<commit_message>
fix rootdepth, doesn't include phenologynow
</commit_message>
<xml_diff>
--- a/data-raw/rootdepth/rd_20200522-maxrootdepth.xlsx
+++ b/data-raw/rootdepth/rd_20200522-maxrootdepth.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnichols\Documents\_github_pkgs\maRsden\data-raw\rootdepth\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gina Laptippytop\Documents\_git_pkgs\maRsden\data-raw\rootdepth\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E400E72A-6F16-446B-B2EF-4F7EC88B1A84}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="root-depth" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>date</t>
   </si>
@@ -58,11 +59,23 @@
   <si>
     <t>Notes: Soil was very wet, corn was very small, only did 2 blocks</t>
   </si>
+  <si>
+    <t>Root depth collected using a regular soil probe in-row adjacent to or between corn plants, 4 per plot</t>
+  </si>
+  <si>
+    <t>ay 22 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gina </t>
+  </si>
+  <si>
+    <t>Soil was very wet, corn was very small, only did 2 blocks</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -403,48 +416,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="4.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.33203125" style="4" customWidth="1"/>
     <col min="9" max="9" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="10" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -464,9 +489,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
-        <v>43642</v>
+        <v>43973</v>
       </c>
       <c r="B7" s="1">
         <v>13</v>
@@ -485,7 +510,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1">
@@ -500,7 +525,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1">
@@ -515,7 +540,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1">
@@ -530,7 +555,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="1">
         <v>17</v>
@@ -547,7 +572,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1">
@@ -562,7 +587,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1">
@@ -577,7 +602,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1">
@@ -592,7 +617,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="1">
         <v>22</v>
@@ -607,7 +632,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1">
@@ -620,7 +645,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1">
@@ -633,7 +658,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1">
@@ -646,7 +671,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="1">
         <v>24</v>
@@ -661,7 +686,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1">
@@ -674,7 +699,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1">
@@ -687,7 +712,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1">
@@ -700,7 +725,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="1">
         <v>34</v>
@@ -717,7 +742,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1">
@@ -732,7 +757,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1">
@@ -747,7 +772,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1">
@@ -762,7 +787,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="1">
         <v>39</v>
@@ -779,7 +804,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1">
@@ -794,7 +819,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1">
@@ -809,7 +834,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1">
@@ -824,7 +849,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="1">
         <v>41</v>
@@ -839,7 +864,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1">
@@ -852,7 +877,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1">
@@ -865,7 +890,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1">
@@ -878,7 +903,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
       <c r="B35" s="1">
         <v>44</v>
@@ -893,7 +918,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1">
@@ -906,7 +931,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1">
@@ -919,7 +944,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1">
@@ -932,7 +957,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -943,7 +968,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -954,7 +979,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -965,7 +990,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -976,7 +1001,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -987,7 +1012,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -998,7 +1023,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1009,7 +1034,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1020,7 +1045,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1031,7 +1056,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1042,7 +1067,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1053,7 +1078,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1064,7 +1089,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1075,7 +1100,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1086,7 +1111,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1097,7 +1122,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1108,7 +1133,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1119,7 +1144,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1130,7 +1155,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1141,7 +1166,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1152,7 +1177,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1163,7 +1188,7 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1174,7 +1199,7 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1185,7 +1210,7 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="6"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1196,7 +1221,7 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1207,7 +1232,7 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1218,7 +1243,7 @@
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="6"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1229,7 +1254,7 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="6"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1240,7 +1265,7 @@
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="6"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1251,7 +1276,7 @@
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="6"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1262,7 +1287,7 @@
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="6"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1273,7 +1298,7 @@
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1284,7 +1309,7 @@
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="6"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1295,7 +1320,7 @@
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="6"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1306,7 +1331,7 @@
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="6"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1317,7 +1342,7 @@
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="6"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1328,7 +1353,7 @@
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="6"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1339,7 +1364,7 @@
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="6"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1350,7 +1375,7 @@
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="6"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1361,7 +1386,7 @@
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="6"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1372,7 +1397,7 @@
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="6"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1383,7 +1408,7 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="6"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1394,7 +1419,7 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="6"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1405,7 +1430,7 @@
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="6"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1416,7 +1441,7 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="6"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1427,7 +1452,7 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="6"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -1438,7 +1463,7 @@
       <c r="H84" s="1"/>
       <c r="I84" s="7"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="6"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1449,7 +1474,7 @@
       <c r="H85" s="1"/>
       <c r="I85" s="7"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="6"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -1460,7 +1485,7 @@
       <c r="H86" s="1"/>
       <c r="I86" s="7"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="6"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -1471,7 +1496,7 @@
       <c r="H87" s="1"/>
       <c r="I87" s="7"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="6"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -1481,7 +1506,7 @@
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="6"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -1491,7 +1516,7 @@
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="6"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -1501,7 +1526,7 @@
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="6"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -1511,7 +1536,7 @@
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="6"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -1521,7 +1546,7 @@
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="6"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -1531,7 +1556,7 @@
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="6"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -1541,7 +1566,7 @@
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="6"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -1551,7 +1576,7 @@
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="6"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -1561,7 +1586,7 @@
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="6"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -1571,7 +1596,7 @@
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="6"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -1581,7 +1606,7 @@
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="6"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -1591,7 +1616,7 @@
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="6"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -1601,7 +1626,7 @@
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="6"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -1611,7 +1636,7 @@
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="6"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -1621,7 +1646,7 @@
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="6"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -1631,7 +1656,7 @@
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="6"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -1641,7 +1666,7 @@
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="6"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -1651,7 +1676,7 @@
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="6"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -1661,7 +1686,7 @@
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="6"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -1671,7 +1696,7 @@
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="6"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -1681,7 +1706,7 @@
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="6"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -1691,7 +1716,7 @@
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="6"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -1701,7 +1726,7 @@
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="6"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -1711,7 +1736,7 @@
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="6"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -1721,7 +1746,7 @@
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="6"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -1731,7 +1756,7 @@
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="6"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -1741,7 +1766,7 @@
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="6"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -1751,7 +1776,7 @@
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="6"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -1761,7 +1786,7 @@
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="6"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -1771,7 +1796,7 @@
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="6"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -1781,7 +1806,7 @@
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="6"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -1791,7 +1816,7 @@
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="6"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -1801,7 +1826,7 @@
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="6"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -1811,7 +1836,7 @@
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="6"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -1821,7 +1846,7 @@
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="6"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -1831,7 +1856,7 @@
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="6"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -1841,7 +1866,7 @@
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="6"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -1851,7 +1876,7 @@
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="6"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -1861,7 +1886,7 @@
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="6"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -1871,7 +1896,7 @@
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="6"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -1881,7 +1906,7 @@
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="6"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -1891,7 +1916,7 @@
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="6"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -1901,7 +1926,7 @@
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="6"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -1911,7 +1936,7 @@
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="6"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -1921,7 +1946,7 @@
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="6"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -1931,7 +1956,7 @@
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="6"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -1941,7 +1966,7 @@
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="6"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -1951,7 +1976,7 @@
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="6"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -1961,7 +1986,7 @@
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="6"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -1971,7 +1996,7 @@
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="6"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -1981,7 +2006,7 @@
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="6"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -1991,7 +2016,7 @@
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="6"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -2001,7 +2026,7 @@
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="6"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -2011,7 +2036,7 @@
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="6"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -2021,7 +2046,7 @@
       <c r="G142" s="2"/>
       <c r="H142" s="1"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" s="6"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -2031,7 +2056,7 @@
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" s="6"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -2041,7 +2066,7 @@
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" s="6"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -2051,7 +2076,7 @@
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" s="6"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -2061,7 +2086,7 @@
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="6"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -2071,7 +2096,7 @@
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="6"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -2081,7 +2106,7 @@
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" s="6"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -2091,7 +2116,7 @@
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" s="6"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -2101,7 +2126,7 @@
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" s="6"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -2111,7 +2136,7 @@
       <c r="G151" s="1"/>
       <c r="H151" s="1"/>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" s="6"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -2121,7 +2146,7 @@
       <c r="G152" s="1"/>
       <c r="H152" s="1"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" s="6"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -2131,7 +2156,7 @@
       <c r="G153" s="1"/>
       <c r="H153" s="1"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" s="6"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -2141,7 +2166,7 @@
       <c r="G154" s="1"/>
       <c r="H154" s="1"/>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" s="6"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -2151,7 +2176,7 @@
       <c r="G155" s="1"/>
       <c r="H155" s="1"/>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" s="6"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -2161,7 +2186,7 @@
       <c r="G156" s="1"/>
       <c r="H156" s="1"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" s="6"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -2171,7 +2196,7 @@
       <c r="G157" s="1"/>
       <c r="H157" s="1"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" s="6"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -2181,7 +2206,7 @@
       <c r="G158" s="2"/>
       <c r="H158" s="1"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" s="6"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -2191,7 +2216,7 @@
       <c r="G159" s="1"/>
       <c r="H159" s="1"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" s="6"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -2201,7 +2226,7 @@
       <c r="G160" s="1"/>
       <c r="H160" s="1"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" s="6"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -2211,7 +2236,7 @@
       <c r="G161" s="1"/>
       <c r="H161" s="1"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" s="6"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -2221,7 +2246,7 @@
       <c r="G162" s="1"/>
       <c r="H162" s="1"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" s="6"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -2231,7 +2256,7 @@
       <c r="G163" s="1"/>
       <c r="H163" s="1"/>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="6"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -2241,7 +2266,7 @@
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" s="6"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -2251,7 +2276,7 @@
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" s="6"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -2261,7 +2286,7 @@
       <c r="G166" s="1"/>
       <c r="H166" s="1"/>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" s="6"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -2271,7 +2296,7 @@
       <c r="G167" s="1"/>
       <c r="H167" s="1"/>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" s="6"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -2281,7 +2306,7 @@
       <c r="G168" s="1"/>
       <c r="H168" s="1"/>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="6"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -2291,7 +2316,7 @@
       <c r="G169" s="1"/>
       <c r="H169" s="1"/>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" s="6"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -2301,7 +2326,7 @@
       <c r="G170" s="1"/>
       <c r="H170" s="1"/>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" s="6"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -2311,7 +2336,7 @@
       <c r="G171" s="1"/>
       <c r="H171" s="1"/>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" s="6"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -2321,7 +2346,7 @@
       <c r="G172" s="1"/>
       <c r="H172" s="1"/>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" s="6"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -2331,7 +2356,7 @@
       <c r="G173" s="1"/>
       <c r="H173" s="1"/>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" s="6"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -2341,7 +2366,7 @@
       <c r="G174" s="3"/>
       <c r="H174" s="1"/>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" s="6"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -2351,7 +2376,7 @@
       <c r="G175" s="1"/>
       <c r="H175" s="1"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" s="6"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -2361,7 +2386,7 @@
       <c r="G176" s="1"/>
       <c r="H176" s="1"/>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" s="6"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -2371,7 +2396,7 @@
       <c r="G177" s="1"/>
       <c r="H177" s="1"/>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" s="6"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -2381,7 +2406,7 @@
       <c r="G178" s="1"/>
       <c r="H178" s="1"/>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" s="6"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -2391,7 +2416,7 @@
       <c r="G179" s="1"/>
       <c r="H179" s="1"/>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" s="6"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -2401,7 +2426,7 @@
       <c r="G180" s="1"/>
       <c r="H180" s="1"/>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" s="6"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -2411,7 +2436,7 @@
       <c r="G181" s="1"/>
       <c r="H181" s="1"/>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" s="6"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -2421,7 +2446,7 @@
       <c r="G182" s="1"/>
       <c r="H182" s="1"/>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" s="6"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -2431,7 +2456,7 @@
       <c r="G183" s="1"/>
       <c r="H183" s="1"/>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184" s="6"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -2441,7 +2466,7 @@
       <c r="G184" s="1"/>
       <c r="H184" s="1"/>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" s="6"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -2451,7 +2476,7 @@
       <c r="G185" s="1"/>
       <c r="H185" s="1"/>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" s="6"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -2461,7 +2486,7 @@
       <c r="G186" s="1"/>
       <c r="H186" s="1"/>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" s="6"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -2471,7 +2496,7 @@
       <c r="G187" s="1"/>
       <c r="H187" s="1"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" s="6"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -2481,7 +2506,7 @@
       <c r="G188" s="1"/>
       <c r="H188" s="1"/>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" s="6"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -2491,7 +2516,7 @@
       <c r="G189" s="1"/>
       <c r="H189" s="1"/>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" s="6"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -2501,7 +2526,7 @@
       <c r="G190" s="3"/>
       <c r="H190" s="1"/>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" s="6"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -2511,7 +2536,7 @@
       <c r="G191" s="1"/>
       <c r="H191" s="1"/>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" s="6"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -2521,7 +2546,7 @@
       <c r="G192" s="1"/>
       <c r="H192" s="1"/>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" s="6"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -2531,7 +2556,7 @@
       <c r="G193" s="1"/>
       <c r="H193" s="1"/>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" s="6"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -2541,7 +2566,7 @@
       <c r="G194" s="1"/>
       <c r="H194" s="1"/>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" s="6"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -2551,7 +2576,7 @@
       <c r="G195" s="1"/>
       <c r="H195" s="1"/>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196" s="6"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -2561,7 +2586,7 @@
       <c r="G196" s="1"/>
       <c r="H196" s="1"/>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197" s="6"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -2571,7 +2596,7 @@
       <c r="G197" s="1"/>
       <c r="H197" s="1"/>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" s="6"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>

</xml_diff>